<commit_message>
correction for HYCOM ocean
</commit_message>
<xml_diff>
--- a/cmip6/models/giss-e2-1-h/cmip6_nasa-giss_giss-e2-1-h_toplevel.xlsx
+++ b/cmip6/models/giss-e2-1-h/cmip6_nasa-giss_giss-e2-1-h_toplevel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaschmid/Desktop/nasa-giss/cmip6/models/giss-e2-1-h/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3582892C-3782-3F47-9964-82DA767BD26C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31DB4DBD-12C3-1A43-9201-BD86F4786909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5940" yWindow="2560" windowWidth="26740" windowHeight="16960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5940" yWindow="2560" windowWidth="26740" windowHeight="16960" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Frontis" sheetId="1" r:id="rId1"/>
@@ -1303,18 +1303,9 @@
     <t xml:space="preserve">Atmosphere, Ocean, Land, Sea ice, Vegetation, Land Ice are all components that are coupled together as described in Kelley et al (2020) and Schmidt et al (2014). </t>
   </si>
   <si>
-    <t>Atmospheric model is tuned for TOA energy balance with PI SST. Some tuning related to low and high clouds for match to climatological radiative fluxes, and gravity wave drag for stratospheric-tropospheric exchange and high latitude SLP.  Full description in Kelley et al (2020).</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
-    <t xml:space="preserve">Atmospheric model independently with PI SST. Ocean mixing within coupled model to reduce OHC drift in PI coupled control. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ocean accepts natural boundary conditions (so water mass, salt, heat) and is mass conserving (not volume conserving). </t>
-  </si>
-  <si>
     <t>All heat fluxes are conserved.</t>
   </si>
   <si>
@@ -1324,24 +1315,15 @@
     <t>Heat, salt and water mass is conserved. Sea ice uses a conservative brine pocket formation (Bitz and Lipscomp, 1999; Schmidt et al, 2004).</t>
   </si>
   <si>
-    <t xml:space="preserve">Rivers carry water mass and heat which is input directly and naturally into the ocean at the river mouth. Net heat/mass imbalance over ice sheets is distributed to ocean using a fixed area mask separately for the NH (around Greenland) and SH (around Antarctic). Effective glacial runoff (ice and heat) is entered into the ocean over the top 700 meters.  </t>
-  </si>
-  <si>
     <t xml:space="preserve">Fresh water is conserved throughout the model (with the very small exception of the chemical source of H2O in the stratosphere from the oxidation of CH4). </t>
   </si>
   <si>
-    <t xml:space="preserve">Precip, evaporation are added/removed from the ocean naturally. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Precip, evaporation is added/removed from soils/lakes/rivers. </t>
   </si>
   <si>
     <t>Precip/sublimation is added/removed from sea ice.</t>
   </si>
   <si>
-    <t xml:space="preserve">River runoff is added to the ocean naturally at the river outlet. Glacial runoff likewise. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Net mass loss from ice sheets (which in the real world would be iceberg calving) is spread around Greenland and Antarctica (independently) to maintain total water mass balance.  </t>
   </si>
   <si>
@@ -1423,7 +1405,25 @@
     <t xml:space="preserve">Heat is conserved in every component and in every flux. </t>
   </si>
   <si>
-    <t xml:space="preserve">Each component and flux transfer is fully water mass conserving. </t>
+    <t>Atmospheric model is tuned for TOA energy balance with PI SST. Some tuning related to low and high clouds for match to climatological radiative fluxes, and gravity wave drag for stratospheric-tropospheric exchange and high latitude SLP.  Full description in Kelley et al (2020). Ocean tuning: (1) varied number of layers in ML to improve ENSO response; (2) varied depth range over which brine plumes generated during freezing are deposited (southern ocean only).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atmospheric model independently with PI SST. </t>
+  </si>
+  <si>
+    <t>Atmosphere and sea ice are fully water mass conserving. In ocean, freshwater fluxes are converted to virtual salt fluxes. Spatially uniform flux corrections are applied to achieve total salt conservation.</t>
+  </si>
+  <si>
+    <t>Flux coupler conserved heat globally.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">River outflow is converted to (negative) salt flux in small region. Negative salinities are set to zero with commensurate changes to the global corrective salt flux. Net heat/mass imbalance over ice sheets is distributed to ocean using a fixed area mask separately for the NH (around Greenland) and SH (around Antarctic). Effective glacial runoff (ice and heat) is entered into the ocean over the top 700 meters.  </t>
+  </si>
+  <si>
+    <t>Precip/evap is added/removed via virtual salt fluxes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">River runoff is added to the ocean as a virtual salt flux. Glacial runoff likewise. </t>
   </si>
 </sst>
 </file>
@@ -1967,7 +1967,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -2004,7 +2004,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="20" x14ac:dyDescent="0.2">
@@ -2133,7 +2133,7 @@
     </row>
     <row r="9" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>419</v>
@@ -2141,10 +2141,10 @@
     </row>
     <row r="10" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -2173,7 +2173,7 @@
     </row>
     <row r="17" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>7</v>
@@ -2181,7 +2181,7 @@
     </row>
     <row r="18" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>230</v>
@@ -2189,7 +2189,7 @@
     </row>
     <row r="19" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>230</v>
@@ -2197,7 +2197,7 @@
     </row>
     <row r="20" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>230</v>
@@ -2224,8 +2224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AH224"/>
   <sheetViews>
-    <sheetView topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="B132" sqref="B132"/>
+    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
+      <selection activeCell="B191" sqref="B191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2270,7 +2270,7 @@
     </row>
     <row r="6" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="11" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2328,7 +2328,7 @@
     </row>
     <row r="16" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="11" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2431,7 +2431,7 @@
     </row>
     <row r="37" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="11" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2455,7 +2455,7 @@
     </row>
     <row r="41" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="11" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2803,7 +2803,7 @@
     </row>
     <row r="100" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B100" s="11" t="s">
-        <v>426</v>
+        <v>460</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2832,7 +2832,7 @@
     </row>
     <row r="105" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B105" s="11" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2861,7 +2861,7 @@
     </row>
     <row r="110" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B110" s="11" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2890,7 +2890,7 @@
     </row>
     <row r="115" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B115" s="11" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2914,7 +2914,7 @@
     </row>
     <row r="119" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B119" s="11" t="s">
-        <v>428</v>
+        <v>461</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2938,7 +2938,7 @@
     </row>
     <row r="123" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B123" s="11" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2980,7 +2980,7 @@
     </row>
     <row r="132" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B132" s="11" t="s">
-        <v>465</v>
+        <v>459</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3009,7 +3009,7 @@
     </row>
     <row r="137" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B137" s="11" t="s">
-        <v>429</v>
+        <v>463</v>
       </c>
     </row>
     <row r="139" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3038,7 +3038,7 @@
     </row>
     <row r="142" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B142" s="11" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3067,7 +3067,7 @@
     </row>
     <row r="147" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B147" s="11" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="149" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3096,7 +3096,7 @@
     </row>
     <row r="152" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B152" s="11" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
     </row>
     <row r="154" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3125,7 +3125,7 @@
     </row>
     <row r="157" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B157" s="11" t="s">
-        <v>433</v>
+        <v>464</v>
       </c>
     </row>
     <row r="160" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3167,7 +3167,7 @@
     </row>
     <row r="166" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B166" s="11" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="168" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3196,7 +3196,7 @@
     </row>
     <row r="171" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B171" s="11" t="s">
-        <v>435</v>
+        <v>465</v>
       </c>
     </row>
     <row r="173" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3225,7 +3225,7 @@
     </row>
     <row r="176" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B176" s="11" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
     </row>
     <row r="178" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3254,7 +3254,7 @@
     </row>
     <row r="181" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B181" s="11" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
     </row>
     <row r="183" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3283,7 +3283,7 @@
     </row>
     <row r="186" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B186" s="11" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
     </row>
     <row r="188" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3312,7 +3312,7 @@
     </row>
     <row r="191" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B191" s="11" t="s">
-        <v>438</v>
+        <v>466</v>
       </c>
     </row>
     <row r="193" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3341,7 +3341,7 @@
     </row>
     <row r="196" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B196" s="11" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
     </row>
     <row r="198" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3370,7 +3370,7 @@
     </row>
     <row r="201" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B201" s="11" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
     </row>
     <row r="203" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3399,7 +3399,7 @@
     </row>
     <row r="206" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B206" s="11" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
     </row>
     <row r="209" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3441,7 +3441,7 @@
     </row>
     <row r="215" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B215" s="11" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
     </row>
     <row r="218" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3483,7 +3483,7 @@
     </row>
     <row r="224" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B224" s="11" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
     </row>
   </sheetData>
@@ -3552,7 +3552,7 @@
     </row>
     <row r="6" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="11" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3581,7 +3581,7 @@
     </row>
     <row r="11" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="11" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3815,7 +3815,7 @@
     </row>
     <row r="41" spans="1:33" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="11" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
     </row>
     <row r="44" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -4023,7 +4023,7 @@
     </row>
     <row r="70" spans="1:33" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B70" s="11" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
     </row>
     <row r="73" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -4141,7 +4141,7 @@
     </row>
     <row r="85" spans="1:33" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B85" s="11" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
     </row>
     <row r="88" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -4272,7 +4272,7 @@
     </row>
     <row r="103" spans="1:33" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B103" s="11" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
     </row>
     <row r="106" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -4480,7 +4480,7 @@
     </row>
     <row r="132" spans="1:33" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B132" s="11" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
     </row>
     <row r="135" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -4570,7 +4570,7 @@
     </row>
     <row r="146" spans="1:33" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B146" s="11" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
     </row>
     <row r="149" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -4660,7 +4660,7 @@
     </row>
     <row r="160" spans="1:33" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B160" s="11" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
     </row>
     <row r="163" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -4776,7 +4776,7 @@
     </row>
     <row r="178" spans="1:33" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B178" s="11" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
     </row>
     <row r="181" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -5028,7 +5028,7 @@
     </row>
     <row r="215" spans="1:33" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B215" s="11" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
     </row>
     <row r="218" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -5490,7 +5490,7 @@
     </row>
     <row r="274" spans="1:33" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B274" s="11" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
     </row>
     <row r="277" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -5606,7 +5606,7 @@
     </row>
     <row r="292" spans="1:32" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B292" s="11" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
     </row>
     <row r="295" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>